<commit_message>
Saving all files before running new metering code
</commit_message>
<xml_diff>
--- a/02_meter_data/gas_comp_clean_su_km.xlsx
+++ b/02_meter_data/gas_comp_clean_su_km.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sea/PycharmProjects/CRF22_Airplanes/02_meter_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2FA069-8FA0-E34F-B698-B8D4EF091C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9DC847-544E-B444-8A5C-4E6F82DD50F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="3660" windowWidth="26840" windowHeight="15940" xr2:uid="{E45264FD-EFD9-2044-BBB3-1AA31ABAFDEB}"/>
+    <workbookView xWindow="1080" yWindow="760" windowWidth="31280" windowHeight="15940" xr2:uid="{E45264FD-EFD9-2044-BBB3-1AA31ABAFDEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -141,10 +141,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy\ hh:mm:ss"/>
     <numFmt numFmtId="166" formatCode="0.0000%"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -194,10 +195,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,7 +517,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:J16"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -572,7 +573,7 @@
       <c r="C2" s="2">
         <v>44839</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>44846.758333333331</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -584,10 +585,10 @@
       <c r="G2" s="1">
         <v>44839</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="6">
         <v>0.94</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="6">
         <v>0.94007708632107823</v>
       </c>
       <c r="J2" s="7">
@@ -604,7 +605,7 @@
       <c r="C3" s="2">
         <v>44846.758333333331</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>44853</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -616,10 +617,10 @@
       <c r="G3" s="1">
         <v>44846</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="6">
         <v>0.92</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="6">
         <v>0.92027516227351991</v>
       </c>
       <c r="J3" s="7">
@@ -636,7 +637,7 @@
       <c r="C4" s="2">
         <v>44853</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>44859.737812500003</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -648,10 +649,10 @@
       <c r="G4" s="1">
         <v>44853</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="6">
         <v>0.9</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="6">
         <v>0.89582545338721564</v>
       </c>
       <c r="J4" s="7">
@@ -668,7 +669,7 @@
       <c r="C5" s="2">
         <v>44859.737812500003</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>44862</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -680,10 +681,10 @@
       <c r="G5" s="1">
         <v>44859</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="6">
         <v>0.88</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="6">
         <v>0.87892770819600086</v>
       </c>
       <c r="J5" s="7">
@@ -700,7 +701,7 @@
       <c r="C6" s="2">
         <v>44862</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>44863.666666666664</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -712,10 +713,10 @@
       <c r="G6" s="1">
         <v>44861</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="6">
         <v>0.87</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="6">
         <v>0.869938670132959</v>
       </c>
       <c r="J6" s="7">
@@ -732,7 +733,7 @@
       <c r="C7" s="2">
         <v>44863.666666666664</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>44865</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -744,10 +745,10 @@
       <c r="G7" s="1">
         <v>44863</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="6">
         <v>0.92</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="6">
         <v>0.91978752908078232</v>
       </c>
       <c r="J7" s="7">
@@ -764,7 +765,7 @@
       <c r="C8" s="2">
         <v>44865</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>44866.666666666664</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -776,10 +777,10 @@
       <c r="G8" s="1">
         <v>44864</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="6">
         <v>0.96</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="6">
         <v>0.93214281042103475</v>
       </c>
       <c r="J8" s="7">
@@ -796,7 +797,7 @@
       <c r="C9" s="2">
         <v>44866.666666666664</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>44873</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -808,10 +809,10 @@
       <c r="G9" s="1">
         <v>44866</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="6">
         <v>0.95499999999999996</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="6">
         <v>0.92708997954088534</v>
       </c>
       <c r="J9" s="7">
@@ -828,7 +829,7 @@
       <c r="C10" s="2">
         <v>44873</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>44874</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -840,10 +841,10 @@
       <c r="G10" s="1">
         <v>44872</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="6">
         <v>1</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="6">
         <v>0.9560384838591216</v>
       </c>
       <c r="J10" s="7">
@@ -860,7 +861,7 @@
       <c r="C11" s="2">
         <v>44874</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>44876</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -872,10 +873,10 @@
       <c r="G11" s="1">
         <v>44873</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="6">
         <v>1</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="6">
         <v>0.95459874953305146</v>
       </c>
       <c r="J11" s="7">
@@ -892,7 +893,7 @@
       <c r="C12" s="2">
         <v>44876</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>44880.705555555556</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -904,10 +905,10 @@
       <c r="G12" s="1">
         <v>44876</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="6">
         <v>1</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="6">
         <v>0.95171928088091129</v>
       </c>
       <c r="J12" s="7">
@@ -924,7 +925,7 @@
       <c r="C13" s="2">
         <v>44880.705555555556</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>44882.782638888886</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -936,10 +937,10 @@
       <c r="G13" s="1">
         <v>44880</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="6">
         <v>1</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="6">
         <v>0.94898329628772693</v>
       </c>
       <c r="J13" s="7">
@@ -956,7 +957,7 @@
       <c r="C14" s="2">
         <v>44882.782638888886</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>44886.666666666664</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -968,10 +969,10 @@
       <c r="G14" s="1">
         <v>44882</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="6">
         <v>1</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="6">
         <v>0.95871133418083021</v>
       </c>
       <c r="J14" s="7">
@@ -988,7 +989,7 @@
       <c r="C15" s="2">
         <v>44886.666666666664</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>44893</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1000,10 +1001,10 @@
       <c r="G15" s="1">
         <v>44884</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="6">
         <v>1</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="6">
         <v>0.94812252990126344</v>
       </c>
       <c r="J15" s="7">
@@ -1020,7 +1021,7 @@
       <c r="C16" s="2">
         <v>44893</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>44896</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -1032,10 +1033,10 @@
       <c r="G16" t="s">
         <v>28</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="6">
         <v>0.99</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="6">
         <v>0.93513912792136544</v>
       </c>
       <c r="J16" s="7">
@@ -1043,49 +1044,49 @@
       </c>
     </row>
     <row r="21" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H21" s="6"/>
+      <c r="H21" s="5"/>
     </row>
     <row r="22" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H22" s="6"/>
+      <c r="H22" s="5"/>
     </row>
     <row r="23" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H23" s="6"/>
+      <c r="H23" s="5"/>
     </row>
     <row r="24" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H24" s="6"/>
+      <c r="H24" s="5"/>
     </row>
     <row r="25" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H25" s="6"/>
+      <c r="H25" s="5"/>
     </row>
     <row r="26" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H26" s="6"/>
+      <c r="H26" s="5"/>
     </row>
     <row r="27" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H27" s="6"/>
+      <c r="H27" s="5"/>
     </row>
     <row r="28" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H28" s="6"/>
+      <c r="H28" s="5"/>
     </row>
     <row r="29" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H29" s="6"/>
+      <c r="H29" s="5"/>
     </row>
     <row r="30" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H30" s="6"/>
+      <c r="H30" s="5"/>
     </row>
     <row r="31" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H31" s="6"/>
+      <c r="H31" s="5"/>
     </row>
     <row r="32" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H32" s="6"/>
+      <c r="H32" s="5"/>
     </row>
     <row r="33" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H33" s="6"/>
+      <c r="H33" s="5"/>
     </row>
     <row r="34" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H34" s="6"/>
+      <c r="H34" s="5"/>
     </row>
     <row r="35" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H35" s="6"/>
+      <c r="H35" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update KM gas composition to include averaged values and standard deviation
</commit_message>
<xml_diff>
--- a/02_meter_data/gas_comp_clean_su_km.xlsx
+++ b/02_meter_data/gas_comp_clean_su_km.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sea/PycharmProjects/CRF22_Airplanes/02_meter_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9DC847-544E-B444-8A5C-4E6F82DD50F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47307779-08E5-F448-A3EE-B38A574E0234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="760" windowWidth="31280" windowHeight="15940" xr2:uid="{E45264FD-EFD9-2044-BBB3-1AA31ABAFDEB}"/>
+    <workbookView xWindow="1060" yWindow="760" windowWidth="31280" windowHeight="15940" xr2:uid="{E45264FD-EFD9-2044-BBB3-1AA31ABAFDEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" iterate="1"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,25 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
-  <si>
-    <t xml:space="preserve">Refill # </t>
-  </si>
-  <si>
-    <t>Rawhide Refill Date</t>
-  </si>
-  <si>
-    <t>Start (UTC)</t>
-  </si>
-  <si>
-    <t>End (UTC)</t>
-  </si>
-  <si>
-    <t>SU Notes</t>
-  </si>
-  <si>
-    <t>KM Composition Date</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>Stop time from log book</t>
   </si>
@@ -113,28 +95,37 @@
     <t>Samples: 24, 25</t>
   </si>
   <si>
-    <t>Missing</t>
-  </si>
-  <si>
-    <t>Thanksgiving refill</t>
-  </si>
-  <si>
     <t>Samples: 26, 27</t>
   </si>
   <si>
-    <t>Missing - average 11/26 and 11/27</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>su_raw</t>
   </si>
   <si>
     <t>su_normalized</t>
   </si>
   <si>
-    <t>km</t>
+    <t>Thanksgiving refill, average 11/26 and 11/27</t>
+  </si>
+  <si>
+    <t>refill_no</t>
+  </si>
+  <si>
+    <t>rawhide_refill_date</t>
+  </si>
+  <si>
+    <t>start_utc</t>
+  </si>
+  <si>
+    <t>end_utc</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>su_notes</t>
+  </si>
+  <si>
+    <t>km_composition_date</t>
   </si>
 </sst>
 </file>
@@ -517,7 +508,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -533,34 +524,31 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
       <c r="H1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -577,10 +565,10 @@
         <v>44846.758333333331</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G2" s="1">
         <v>44839</v>
@@ -591,9 +579,7 @@
       <c r="I2" s="6">
         <v>0.94007708632107823</v>
       </c>
-      <c r="J2" s="7">
-        <v>0.93811800000000001</v>
-      </c>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -609,10 +595,10 @@
         <v>44853</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G3" s="1">
         <v>44846</v>
@@ -623,9 +609,7 @@
       <c r="I3" s="6">
         <v>0.92027516227351991</v>
       </c>
-      <c r="J3" s="7">
-        <v>0.93923199999999996</v>
-      </c>
+      <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -641,10 +625,10 @@
         <v>44859.737812500003</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G4" s="1">
         <v>44853</v>
@@ -655,9 +639,7 @@
       <c r="I4" s="6">
         <v>0.89582545338721564</v>
       </c>
-      <c r="J4" s="7">
-        <v>0.94677199999999995</v>
-      </c>
+      <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -673,10 +655,10 @@
         <v>44862</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G5" s="1">
         <v>44859</v>
@@ -687,9 +669,7 @@
       <c r="I5" s="6">
         <v>0.87892770819600086</v>
       </c>
-      <c r="J5" s="7">
-        <v>0.94872100000000004</v>
-      </c>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -705,10 +685,10 @@
         <v>44863.666666666664</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G6" s="1">
         <v>44861</v>
@@ -719,9 +699,7 @@
       <c r="I6" s="6">
         <v>0.869938670132959</v>
       </c>
-      <c r="J6" s="7">
-        <v>0.95966300000000004</v>
-      </c>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -737,10 +715,10 @@
         <v>44865</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G7" s="1">
         <v>44863</v>
@@ -751,9 +729,7 @@
       <c r="I7" s="6">
         <v>0.91978752908078232</v>
       </c>
-      <c r="J7" s="7">
-        <v>0.95136100000000001</v>
-      </c>
+      <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -769,10 +745,10 @@
         <v>44866.666666666664</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1">
         <v>44864</v>
@@ -783,9 +759,7 @@
       <c r="I8" s="6">
         <v>0.93214281042103475</v>
       </c>
-      <c r="J8" s="7">
-        <v>0.94901300000000011</v>
-      </c>
+      <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -801,10 +775,10 @@
         <v>44873</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G9" s="1">
         <v>44866</v>
@@ -815,9 +789,7 @@
       <c r="I9" s="6">
         <v>0.92708997954088534</v>
       </c>
-      <c r="J9" s="7">
-        <v>0.94561600000000001</v>
-      </c>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -833,10 +805,10 @@
         <v>44874</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
         <v>12</v>
-      </c>
-      <c r="F10" t="s">
-        <v>18</v>
       </c>
       <c r="G10" s="1">
         <v>44872</v>
@@ -847,9 +819,7 @@
       <c r="I10" s="6">
         <v>0.9560384838591216</v>
       </c>
-      <c r="J10" s="7">
-        <v>0.95586299999999991</v>
-      </c>
+      <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -865,10 +835,10 @@
         <v>44876</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G11" s="1">
         <v>44873</v>
@@ -879,9 +849,7 @@
       <c r="I11" s="6">
         <v>0.95459874953305146</v>
       </c>
-      <c r="J11" s="7">
-        <v>0.95365999999999995</v>
-      </c>
+      <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -897,10 +865,10 @@
         <v>44880.705555555556</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G12" s="1">
         <v>44876</v>
@@ -911,9 +879,7 @@
       <c r="I12" s="6">
         <v>0.95171928088091129</v>
       </c>
-      <c r="J12" s="7">
-        <v>0.95074100000000006</v>
-      </c>
+      <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -929,10 +895,10 @@
         <v>44882.782638888886</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G13" s="1">
         <v>44880</v>
@@ -943,9 +909,7 @@
       <c r="I13" s="6">
         <v>0.94898329628772693</v>
       </c>
-      <c r="J13" s="7">
-        <v>0.94182500000000002</v>
-      </c>
+      <c r="J13" s="7"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -961,10 +925,10 @@
         <v>44886.666666666664</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F14" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G14" s="1">
         <v>44882</v>
@@ -975,9 +939,7 @@
       <c r="I14" s="6">
         <v>0.95871133418083021</v>
       </c>
-      <c r="J14" s="7">
-        <v>0.94035799999999992</v>
-      </c>
+      <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -993,10 +955,10 @@
         <v>44893</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F15" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G15" s="1">
         <v>44884</v>
@@ -1007,16 +969,14 @@
       <c r="I15" s="6">
         <v>0.94812252990126344</v>
       </c>
-      <c r="J15" s="7">
-        <v>0.94150400000000001</v>
-      </c>
+      <c r="J15" s="7"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>25</v>
+      <c r="B16" s="1">
+        <v>44891</v>
       </c>
       <c r="C16" s="2">
         <v>44893</v>
@@ -1025,13 +985,13 @@
         <v>44896</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F16" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" t="s">
-        <v>28</v>
+        <v>19</v>
+      </c>
+      <c r="G16" s="1">
+        <v>44891</v>
       </c>
       <c r="H16" s="6">
         <v>0.99</v>
@@ -1039,9 +999,7 @@
       <c r="I16" s="6">
         <v>0.93513912792136544</v>
       </c>
-      <c r="J16" s="7">
-        <v>0.94193749999999998</v>
-      </c>
+      <c r="J16" s="7"/>
     </row>
     <row r="21" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H21" s="5"/>

</xml_diff>